<commit_message>
Updates to lean canvas
There were some embarrassing typo's and older mentions of previous name which is not correct.
</commit_message>
<xml_diff>
--- a/whats-left/whatsleft_ lean_canvas_v1.xlsx
+++ b/whats-left/whatsleft_ lean_canvas_v1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Whatsleft - lean canvas</t>
   </si>
@@ -37,23 +37,25 @@
     <t>Customer segments</t>
   </si>
   <si>
-    <t>Small businesses - eg sole proprietors, partnerships - don't have a real-time image of their true available funds: the GST they owe after income and expenses, and what their accurate, real-time available funds are.</t>
+    <t>Small businesses - eg sole proprietors, partnerships - don't have an idea of their available balance right now. Their internet banking says $100, but that's not a real-time image of their true available funds, i.e. considering the GST they owe after income and expenses.</t>
   </si>
   <si>
-    <t>GST-as-a-service:
+    <t>Cashflow-as-a-service:
  - accurate, real-time available funds, calculated as funds in account minus GST, outgoings etc
  - forecast GST payable
  - reminders when GST is due</t>
   </si>
   <si>
-    <t>There are no Personal Finance Manager (PFM) products for small businesses at the moment. The products in the market currently address forecasting tools and larger financial obiligations.
-There are for consumers - eg Kiwibank's beta service (still in testing) - and large organisations will use accountants etc.</t>
+    <t>There are no Personal Finance Manager (PFM) products for small businesses at the moment which address this critical but simple focus. The products in the market currently address forecasting tools and larger financial obiligations.</t>
   </si>
   <si>
     <t>We have the data for this kind of thing (ito business analysis), and might find it easier than many to set up the relationship with IR.</t>
   </si>
   <si>
-    <t xml:space="preserve">Small organisations with simple finances (1-10 people).with revenues of $60 - 500k /annum </t>
+    <t xml:space="preserve">Small organisations with simple finances (1-10 people) with revenues of $60 - 500k /annum </t>
+  </si>
+  <si>
+    <t>Businesses this size generally have an accountant/bookkeeper that does their year end, and occasionally their GST. Only then, do they know their cash position.</t>
   </si>
   <si>
     <t xml:space="preserve">Owner operators </t>
@@ -83,8 +85,7 @@
     <t>IRD metric on paying GST on time</t>
   </si>
   <si>
-    <t>Personal finance management (PFM) for small businesses, giving a real-time picture of their GST commitments and what funds they truly have available.
-No accountants needed (for your GST)!</t>
+    <t>Personal finance management (PFM) for small businesses giving a real-time picture of their available bank balance considering the incoming and outgoing of day to day business tax commitments.</t>
   </si>
   <si>
     <t>Social networks.</t>
@@ -96,9 +97,6 @@
     <t>Accountants.</t>
   </si>
   <si>
-    <t xml:space="preserve">Stakeholders </t>
-  </si>
-  <si>
     <t>Word of mouth.</t>
   </si>
   <si>
@@ -108,16 +106,10 @@
     <t>Bookkeepers</t>
   </si>
   <si>
-    <t xml:space="preserve">Technology development partner </t>
-  </si>
-  <si>
     <t>BAnks - Westpac, Asb (MVP)</t>
   </si>
   <si>
     <t>Henry.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Branding and website </t>
   </si>
   <si>
     <t>MYOB / Xero customers.</t>
@@ -126,16 +118,10 @@
     <t>Bosspac.</t>
   </si>
   <si>
-    <t>Central gvt agency</t>
-  </si>
-  <si>
     <t>Small business consultances / services / advice organisations / services / directories (eg the wellington business support tool).</t>
   </si>
   <si>
     <t>Assumptions :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accountants </t>
   </si>
   <si>
     <t>Training or advice for people starting out/small businesses.</t>
@@ -150,28 +136,28 @@
     <t>Revenue streams</t>
   </si>
   <si>
-    <t>Complexity: 3</t>
+    <t>Complexity: 3 - We have considered the data sets required to make this happen</t>
   </si>
   <si>
     <t>Subscribers to the app / API.</t>
   </si>
   <si>
-    <t>Risk: 5</t>
+    <t>Risk: 5 - Reputation, security and financial risk are at an acceptable level. We have considered the risks and are confident we can mitigate the associated risk.</t>
   </si>
   <si>
     <t xml:space="preserve">A cut if the app / API gets people to sign onto accounting products </t>
   </si>
   <si>
-    <t>Effort: 5</t>
+    <t>Effort: 5 - The effort is relatively simple based on what we know, and have a good idea of the work required.</t>
   </si>
   <si>
     <t>White labelling / license fees for organisations like banks?</t>
   </si>
   <si>
-    <t>Acquisition: 5 Customers</t>
+    <t>Acquisition: 2 - Data sets required are available, not in an ideal state but good enough to get a first offering out.</t>
   </si>
   <si>
-    <t xml:space="preserve">Value (1 = lowest): 7 </t>
+    <t>Value: 7 - There is an untapped value for young business owners/contractors not being serviced by accountants, bookkeepers or accounting products.</t>
   </si>
 </sst>
 </file>
@@ -375,15 +361,15 @@
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -457,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -574,17 +560,17 @@
       <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="12" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="5"/>
@@ -609,13 +595,15 @@
       <c r="Z4" s="6"/>
     </row>
     <row r="5">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="14"/>
       <c r="C5" s="15"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12" t="s">
-        <v>13</v>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -639,13 +627,13 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="15"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="11"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
       <c r="F6" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -669,11 +657,11 @@
       <c r="Z6" s="6"/>
     </row>
     <row r="7">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="15"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="17"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -698,20 +686,20 @@
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="20" t="s">
         <v>18</v>
       </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="F8" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -735,21 +723,21 @@
       <c r="Z8" s="6"/>
     </row>
     <row r="9" ht="87.75" customHeight="1">
-      <c r="A9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14" t="s">
         <v>24</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -773,18 +761,16 @@
       <c r="Z9" s="6"/>
     </row>
     <row r="10">
-      <c r="A10" s="11" t="s">
-        <v>25</v>
+      <c r="A10" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="14"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="5"/>
@@ -809,18 +795,16 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="15"/>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="12"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -843,18 +827,16 @@
       <c r="Z11" s="6"/>
     </row>
     <row r="12">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -877,18 +859,16 @@
       <c r="Z12" s="6"/>
     </row>
     <row r="13">
-      <c r="A13" s="12" t="s">
-        <v>35</v>
+      <c r="A13" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="B13" s="15"/>
-      <c r="C13" s="22" t="s">
-        <v>36</v>
-      </c>
+      <c r="C13" s="22"/>
       <c r="D13" s="23"/>
       <c r="E13" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -912,17 +892,15 @@
     </row>
     <row r="14">
       <c r="A14" s="24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="22" t="s">
-        <v>39</v>
+      <c r="B14" s="14"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="11" t="s">
+        <v>36</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="11"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -950,7 +928,7 @@
       <c r="C15" s="26"/>
       <c r="D15" s="27"/>
       <c r="E15" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="5"/>
@@ -976,12 +954,12 @@
     </row>
     <row r="16" ht="22.5" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="9"/>
       <c r="D16" s="30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="9"/>
@@ -1008,13 +986,13 @@
     </row>
     <row r="17">
       <c r="A17" s="31" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
-      <c r="C17" s="14"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
-      <c r="F17" s="14"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1038,13 +1016,13 @@
     </row>
     <row r="18">
       <c r="A18" s="31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
-      <c r="F18" s="14"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1068,13 +1046,13 @@
     </row>
     <row r="19">
       <c r="A19" s="31" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
-      <c r="C19" s="14"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
-      <c r="F19" s="14"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1098,11 +1076,11 @@
     </row>
     <row r="20">
       <c r="A20" s="31" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="5"/>
-      <c r="F20" s="14"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1126,7 +1104,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="33" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="27"/>
@@ -1155,7 +1133,7 @@
       <c r="Z21" s="6"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="5"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="4"/>
@@ -1211,7 +1189,7 @@
       <c r="Z23" s="6"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="6"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1239,7 +1217,7 @@
       <c r="Z24" s="6"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="6"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1267,7 +1245,7 @@
       <c r="Z25" s="6"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="6"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1295,7 +1273,7 @@
       <c r="Z26" s="6"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="6"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1323,7 +1301,7 @@
       <c r="Z27" s="6"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="6"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -1351,7 +1329,7 @@
       <c r="Z28" s="6"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="6"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -1379,7 +1357,7 @@
       <c r="Z29" s="6"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="6"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1407,7 +1385,7 @@
       <c r="Z30" s="6"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="6"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -28592,8 +28570,8 @@
     <mergeCell ref="C9:D9"/>
   </mergeCells>
   <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="1.0" right="1.0" top="0.75"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>